<commit_message>
Update the schema.sql and data.sql per the code table spread sheet and ER-D changes.
</commit_message>
<xml_diff>
--- a/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTables.xlsx
+++ b/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22100" yWindow="1380" windowWidth="20480" windowHeight="12400" tabRatio="705" firstSheet="27" activeTab="29"/>
+    <workbookView xWindow="1620" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="705" firstSheet="25" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="655">
   <si>
     <t>Table</t>
   </si>
@@ -1940,9 +1940,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>98</t>
-  </si>
-  <si>
     <t>Covered by another agency</t>
   </si>
   <si>
@@ -2013,6 +2010,9 @@
   </si>
   <si>
     <t>Blank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -2067,9 +2067,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2097,7 +2109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="28">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2105,6 +2117,12 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2112,6 +2130,12 @@
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
@@ -2658,10 +2682,10 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B30" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
   </sheetData>
@@ -2683,7 +2707,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3086,7 +3110,7 @@
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1">
       <c r="A29" s="1">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B29">
         <v>99</v>
@@ -3100,16 +3124,16 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B30" t="s">
+        <v>652</v>
+      </c>
+      <c r="C30" t="s">
         <v>653</v>
       </c>
-      <c r="C30" t="s">
-        <v>654</v>
-      </c>
       <c r="D30" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -3128,7 +3152,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3227,10 +3251,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1">
       <c r="A9">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>525</v>
+        <v>629</v>
       </c>
       <c r="C9" t="s">
         <v>274</v>
@@ -3238,13 +3262,13 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C10" t="s">
         <v>653</v>
-      </c>
-      <c r="C10" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -3263,7 +3287,7 @@
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4023,7 +4047,7 @@
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1">
       <c r="A69">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>345</v>
@@ -4034,13 +4058,13 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>98</v>
+        <v>99998</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>630</v>
+        <v>652</v>
       </c>
       <c r="C70" t="s">
-        <v>275</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -4059,7 +4083,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4257,7 +4281,7 @@
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B18" t="s">
         <v>255</v>
@@ -4279,13 +4303,13 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>98</v>
+        <v>99998</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>629</v>
+        <v>652</v>
       </c>
       <c r="C20" t="s">
-        <v>275</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -4301,10 +4325,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4446,7 +4470,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>345</v>
@@ -4457,24 +4481,13 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>98</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>630</v>
+        <v>99998</v>
+      </c>
+      <c r="B14" t="s">
+        <v>652</v>
       </c>
       <c r="C14" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>99999</v>
-      </c>
-      <c r="B15" t="s">
         <v>653</v>
-      </c>
-      <c r="C15" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -4493,7 +4506,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4602,7 +4615,7 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1">
       <c r="A10">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B10" t="s">
         <v>255</v>
@@ -4613,13 +4626,13 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B11" t="s">
+        <v>652</v>
+      </c>
+      <c r="C11" t="s">
         <v>653</v>
-      </c>
-      <c r="C11" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -4638,7 +4651,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4780,7 +4793,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>345</v>
@@ -4791,13 +4804,13 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B14" t="s">
+        <v>652</v>
+      </c>
+      <c r="C14" t="s">
         <v>653</v>
-      </c>
-      <c r="C14" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -4816,7 +4829,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4914,7 +4927,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>525</v>
@@ -4925,13 +4938,13 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B10" t="s">
+        <v>652</v>
+      </c>
+      <c r="C10" t="s">
         <v>653</v>
-      </c>
-      <c r="C10" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -4950,7 +4963,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4990,7 +5003,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1">
       <c r="A4">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B4" t="s">
         <v>255</v>
@@ -5001,13 +5014,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B5" t="s">
+        <v>652</v>
+      </c>
+      <c r="C5" t="s">
         <v>653</v>
-      </c>
-      <c r="C5" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5026,7 +5039,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5102,7 +5115,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1">
       <c r="A7">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B7" t="s">
         <v>255</v>
@@ -5113,13 +5126,13 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B8" t="s">
+        <v>652</v>
+      </c>
+      <c r="C8" t="s">
         <v>653</v>
-      </c>
-      <c r="C8" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5141,7 +5154,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5217,7 +5230,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>525</v>
@@ -5228,13 +5241,13 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B8" t="s">
+        <v>652</v>
+      </c>
+      <c r="C8" t="s">
         <v>653</v>
-      </c>
-      <c r="C8" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5253,7 +5266,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5293,7 +5306,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1">
       <c r="A4">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B4" t="s">
         <v>255</v>
@@ -5304,13 +5317,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B5" t="s">
+        <v>652</v>
+      </c>
+      <c r="C5" t="s">
         <v>653</v>
-      </c>
-      <c r="C5" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5329,7 +5342,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5369,7 +5382,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1">
       <c r="A4">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B4" t="s">
         <v>255</v>
@@ -5380,13 +5393,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B5" t="s">
+        <v>652</v>
+      </c>
+      <c r="C5" t="s">
         <v>653</v>
-      </c>
-      <c r="C5" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5402,10 +5415,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5613,7 +5626,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>345</v>
@@ -5624,24 +5637,13 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>98</v>
+        <v>99998</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>630</v>
+        <v>652</v>
       </c>
       <c r="C20" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>99999</v>
-      </c>
-      <c r="B21" t="s">
         <v>653</v>
-      </c>
-      <c r="C21" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5660,7 +5662,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5758,29 +5760,29 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>525</v>
+        <v>99998</v>
+      </c>
+      <c r="B9" t="s">
+        <v>652</v>
       </c>
       <c r="C9" t="s">
-        <v>274</v>
+        <v>653</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
         <v>99999</v>
       </c>
-      <c r="B10" t="s">
-        <v>653</v>
+      <c r="B10" s="6" t="s">
+        <v>525</v>
       </c>
       <c r="C10" t="s">
-        <v>654</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5794,7 +5796,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5903,29 +5905,29 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>525</v>
+        <v>99998</v>
+      </c>
+      <c r="B10" t="s">
+        <v>652</v>
       </c>
       <c r="C10" t="s">
-        <v>274</v>
+        <v>653</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
         <v>99999</v>
       </c>
-      <c r="B11" t="s">
-        <v>653</v>
+      <c r="B11" s="6" t="s">
+        <v>525</v>
       </c>
       <c r="C11" t="s">
-        <v>654</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5936,10 +5938,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6235,7 +6237,7 @@
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1">
       <c r="A27">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B27" t="s">
         <v>459</v>
@@ -6246,24 +6248,13 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>98</v>
+        <v>99998</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>630</v>
+        <v>654</v>
       </c>
       <c r="C28" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29">
-        <v>99999</v>
-      </c>
-      <c r="B29" t="s">
         <v>653</v>
-      </c>
-      <c r="C29" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -6284,8 +6275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6337,31 +6328,31 @@
         <v>501</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>525</v>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="1">
+        <v>99998</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>652</v>
       </c>
       <c r="C5" t="s">
-        <v>274</v>
+        <v>653</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
         <v>99999</v>
       </c>
-      <c r="B6" t="s">
-        <v>653</v>
+      <c r="B6" s="6" t="s">
+        <v>525</v>
       </c>
       <c r="C6" t="s">
-        <v>654</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6375,7 +6366,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6429,13 +6420,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B5" t="s">
+        <v>652</v>
+      </c>
+      <c r="C5" t="s">
         <v>653</v>
-      </c>
-      <c r="C5" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -6454,7 +6445,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6547,7 +6538,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1">
@@ -6563,29 +6554,29 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>999</v>
+        <v>99998</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>345</v>
+        <v>652</v>
       </c>
       <c r="C10" t="s">
-        <v>274</v>
+        <v>653</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
         <v>99999</v>
       </c>
-      <c r="B11" t="s">
-        <v>653</v>
+      <c r="B11" s="6" t="s">
+        <v>345</v>
       </c>
       <c r="C11" t="s">
-        <v>654</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6599,7 +6590,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6642,29 +6633,29 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>9</v>
+        <v>99998</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>525</v>
+        <v>652</v>
       </c>
       <c r="C4" t="s">
-        <v>274</v>
+        <v>653</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
         <v>99999</v>
       </c>
-      <c r="B5" t="s">
-        <v>653</v>
+      <c r="B5" s="3">
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>654</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6678,7 +6669,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6765,7 +6756,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>525</v>
@@ -6776,13 +6767,13 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B9" t="s">
+        <v>652</v>
+      </c>
+      <c r="C9" t="s">
         <v>653</v>
-      </c>
-      <c r="C9" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -6798,10 +6789,10 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6826,10 +6817,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -6837,10 +6828,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -6848,10 +6839,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -6859,10 +6850,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C5" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6870,10 +6861,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -6881,10 +6872,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -6892,10 +6883,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C8" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -6903,10 +6894,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C9" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -6917,17 +6908,28 @@
         <v>629</v>
       </c>
       <c r="C10" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>99</v>
+        <v>638</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="1" customFormat="1">
+      <c r="A11" s="1">
+        <v>99998</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>99999</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>274</v>
       </c>
     </row>
@@ -6946,7 +6948,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6990,7 +6992,7 @@
         <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D2" t="s">
         <v>494</v>
@@ -6999,7 +7001,7 @@
         <v>496</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G2" t="s">
         <v>521</v>
@@ -7013,7 +7015,7 @@
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>494</v>
@@ -7022,7 +7024,7 @@
         <v>273</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>521</v>
@@ -7036,7 +7038,7 @@
         <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>494</v>
@@ -7045,7 +7047,7 @@
         <v>273</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>522</v>
@@ -8410,7 +8412,7 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64">
-        <v>999</v>
+        <v>99999</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>519</v>
@@ -8433,25 +8435,25 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C65" t="s">
         <v>653</v>
       </c>
-      <c r="C65" t="s">
-        <v>654</v>
-      </c>
       <c r="D65" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E65" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F65" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G65" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -8470,10 +8472,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8538,13 +8540,24 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>525</v>
       </c>
       <c r="C6" t="s">
-        <v>275</v>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>99998</v>
+      </c>
+      <c r="B7" t="s">
+        <v>652</v>
+      </c>
+      <c r="C7" t="s">
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -8562,8 +8575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView topLeftCell="C30" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9080,7 +9093,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>345</v>
@@ -9091,13 +9104,13 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C48" t="s">
         <v>653</v>
-      </c>
-      <c r="C48" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -9116,7 +9129,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9159,7 +9172,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>525</v>
@@ -9170,13 +9183,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B5" t="s">
+        <v>652</v>
+      </c>
+      <c r="C5" t="s">
         <v>653</v>
-      </c>
-      <c r="C5" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -9195,7 +9208,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9337,7 +9350,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>525</v>
@@ -9348,13 +9361,13 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B14" t="s">
+        <v>652</v>
+      </c>
+      <c r="C14" t="s">
         <v>653</v>
-      </c>
-      <c r="C14" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -9373,7 +9386,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9559,7 +9572,7 @@
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17">
-        <v>999</v>
+        <v>99999</v>
       </c>
       <c r="B17" s="2">
         <v>95</v>
@@ -9570,13 +9583,13 @@
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18">
-        <v>990</v>
-      </c>
-      <c r="B18" s="2">
-        <v>99</v>
+        <v>99998</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>652</v>
       </c>
       <c r="C18" t="s">
-        <v>275</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>